<commit_message>
updating plots and text
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">cluster</t>
   </si>
@@ -26,34 +26,40 @@
     <t xml:space="preserve">countries</t>
   </si>
   <si>
+    <t xml:space="preserve">co2_frac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pop_frac</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">Algeria; Azerbaijan; Egypt; Iran (Islamic Republic of); Iraq; Kuwait; Kyrgyzstan; Libya; Mozambique; Saudi Arabia; Uzbekistan; Venezuela (Bolivarian Republic of); Zambia; Zimbabwe</t>
+    <t xml:space="preserve">Algeria; Azerbaijan; Egypt; Iran (Islamic Republic of); Iraq; Kuwait; Libya; Saudi Arabia; Uzbekistan; Venezuela (Bolivarian Republic of); Zimbabwe</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">Argentina; Belarus; Brazil; Colombia; Costa Rica; Ecuador; Hungary; Indonesia; Italy; Mexico; Peru; Philippines; Portugal; Romania; Slovakia; Spain; Thailand; Uruguay</t>
+    <t xml:space="preserve">Argentina; Belarus; Brazil; Chile; Colombia; Costa Rica; Cyprus; Czechia; Ecuador; Estonia; Greece; Hungary; Latvia; Lithuania; Peru; Portugal; Romania; Slovakia; Slovenia; Trinidad and Tobago; Uruguay</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">Armenia; Bangladesh; Benin; Bolivia (Plurinational State of); Cameroon; Cyprus; Dominican Republic; El Salvador; Ghana; Guatemala; Haiti; Honduras; Jordan; Kenya; Lebanon; Malaysia; Morocco; Namibia; Nicaragua; Nigeria; Pakistan; Panama; Paraguay; Republic of Moldova; Senegal; Togo; Tunisia; United Republic of Tanzania; Yemen</t>
+    <t xml:space="preserve">Armenia; Bangladesh; Benin; Bolivia (Plurinational State of); Cameroon; Dominican Republic; El Salvador; Ghana; Guatemala; Haiti; Honduras; Jordan; Kenya; Lebanon; Mexico; Morocco; Mozambique; Namibia; Nicaragua; Nigeria; Pakistan; Panama; Paraguay; Philippines; Republic of Moldova; Senegal; Togo; Tunisia; United Republic of Tanzania; Yemen; Zambia</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">Australia; Austria; Belgium; Canada; Chile; Denmark; Estonia; Finland; France; Germany; Ireland; Japan; Latvia; Lithuania; Netherlands; New Zealand; Norway; Singapore; Slovenia; Sweden; United Kingdom; United States of America</t>
+    <t xml:space="preserve">Australia; Austria; Belgium; Canada; Denmark; Finland; France; Germany; Ireland; Israel; Italy; Japan; Netherlands; New Zealand; Norway; Republic of Korea; Singapore; Spain; Sweden; United Kingdom; United States of America</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">Botswana; Bulgaria; China; Czechia; Greece; India; Israel; Kazakhstan; Poland; Republic of Korea; Russian Federation; South Africa; Trinidad and Tobago; Turkey; Ukraine; Viet Nam</t>
+    <t xml:space="preserve">Botswana; Bulgaria; China; India; Indonesia; Kazakhstan; Kyrgyzstan; Malaysia; Poland; Russian Federation; South Africa; Thailand; Turkey; Ukraine; Viet Nam</t>
   </si>
 </sst>
 </file>
@@ -398,75 +404,111 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0653164411944704</v>
+        <v>2335948737.37047</v>
       </c>
       <c r="C2" t="n">
-        <v>0.058913363542848</v>
+        <v>392003255</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0646123926604703</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0519191585346528</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0894844583090047</v>
+        <v>1534383742.08168</v>
       </c>
       <c r="C3" t="n">
-        <v>0.144001444116225</v>
+        <v>465035220</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0424410875329496</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0615919306878642</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0276915111711873</v>
+        <v>1371971004.98803</v>
       </c>
       <c r="C4" t="n">
-        <v>0.127598620698532</v>
+        <v>1211443545</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0379487477079031</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.160450528576955</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" t="n">
-        <v>0.270566127821201</v>
+        <v>10961791460.5727</v>
       </c>
       <c r="C5" t="n">
-        <v>0.110119123267241</v>
+        <v>970161945</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.303203389176253</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.128493810151505</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>0.467367572104294</v>
+        <v>17072311056.5041</v>
       </c>
       <c r="C6" t="n">
-        <v>0.439470257139885</v>
+        <v>3606362917</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.472220493522581</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.477647380813754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>